<commit_message>
feat: biocatalysis demo vocabulary v1.1
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -1448,25 +1448,7 @@
     <t xml:space="preserve">Source Vocab URI</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">0000001</t>
-    </r>
+    <t xml:space="preserve">v4c-bc:0000001</t>
   </si>
   <si>
     <t xml:space="preserve">Protein</t>
@@ -1559,7 +1541,7 @@
     <t xml:space="preserve">Provenance</t>
   </si>
   <si>
-    <t xml:space="preserve">V4c-bc:0000010</t>
+    <t xml:space="preserve">v4c-bc:0000010</t>
   </si>
   <si>
     <t xml:space="preserve">biocatalysis</t>
@@ -1568,7 +1550,54 @@
     <t xml:space="preserve">Collection of terms related to biocatalysis.</t>
   </si>
   <si>
-    <t xml:space="preserve">ext:0000001, ext:0000002, ext:0000003</t>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">v4c-bc:0000001, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">v4c-bc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:0000002, </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve">v4c-bc</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color rgb="FF000000"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">:0000003</t>
+    </r>
   </si>
   <si>
     <t xml:space="preserve">https://orcid.org/0000-0001-2345-9999 Created collection</t>
@@ -1595,7 +1624,7 @@
     <t xml:space="preserve">v4c-bc</t>
   </si>
   <si>
-    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_biocatalysis/</t>
+    <t xml:space="preserve">https://example.org/voc4cat_biocatalysis/</t>
   </si>
 </sst>
 </file>
@@ -1606,7 +1635,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="21">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1745,13 +1774,6 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <u val="single"/>
-      <sz val="11"/>
-      <color rgb="FF0563C1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -2000,7 +2022,7 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="20" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2180,9 +2202,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>580320</xdr:colOff>
+      <xdr:colOff>579960</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2196,8 +2218,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1375200" y="304920"/>
-          <a:ext cx="5914440" cy="1542600"/>
+          <a:off x="1375920" y="304920"/>
+          <a:ext cx="5917320" cy="1542240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2277,7 +2299,7 @@
       <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2460,7 +2482,7 @@
       <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -5179,7 +5201,7 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -6328,7 +6350,7 @@
     <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999"/>
+    <hyperlink ref="B10" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999 mark doerr"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -6351,7 +6373,7 @@
       <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6675,7 +6697,7 @@
       <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -7217,11 +7239,11 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E4" activeCellId="0" sqref="E4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -7252,7 +7274,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
         <v>112</v>
       </c>
@@ -7390,7 +7412,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999 Created collection"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7412,11 +7434,11 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
@@ -7508,7 +7530,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://example.org/test/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://w3id.org/nfdi4cat/voc4cat_"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_biocatalysis/"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://example.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
feat: new biocatalysis_demo sheet submitted, based on current template
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="6"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -78,12 +78,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="123">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.4</t>
+    <t xml:space="preserve">0.4.3</t>
   </si>
   <si>
     <t xml:space="preserve">revision</t>
@@ -388,7 +388,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
 </t>
     </r>
     <r>
@@ -410,7 +410,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
 </t>
     </r>
     <r>
@@ -422,7 +422,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Note: Either the abbreviation for an organisation or its URI can be given. The organisation abbreviation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).
+      <t xml:space="preserve">Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).
 </t>
     </r>
     <r>
@@ -581,7 +581,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organisation system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
+      <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organization system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
 </t>
     </r>
     <r>
@@ -1237,7 +1237,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+      <t xml:space="preserve">This sheet is for defining a mapping between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
 Example: http://example.org/1, http://example.org/2, http://example.org/3</t>
     </r>
     <r>
@@ -1259,7 +1259,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Instead of manually typing out these examples, you can add in the Prefix Sheet a "ex" as Prefix, and "http://example.org/" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and "http://example.org/" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
 </t>
     </r>
     <r>
@@ -1271,7 +1271,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE, a colon is used to separate the prefix from the suffix-part of the IRI.</t>
+      <t xml:space="preserve">Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE a colon is used to separate the prefix from the suffix-part of the IRI.</t>
     </r>
   </si>
   <si>
@@ -1316,7 +1316,7 @@
     <t xml:space="preserve">Vocabulary IRI*</t>
   </si>
   <si>
-    <t xml:space="preserve">V4c-bc</t>
+    <t xml:space="preserve">v4c-bc</t>
   </si>
   <si>
     <t xml:space="preserve">IRI or CURIE for this vocabulary</t>
@@ -1349,7 +1349,7 @@
     <t xml:space="preserve">Created Date*</t>
   </si>
   <si>
-    <t xml:space="preserve">2023/12/12</t>
+    <t xml:space="preserve">2024/02/20</t>
   </si>
   <si>
     <t xml:space="preserve">Date of creation</t>
@@ -1385,7 +1385,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">V2023-12-12</t>
+    <t xml:space="preserve">V2024-02-20</t>
   </si>
   <si>
     <t xml:space="preserve">Version specifier for the vocabulary (or empty cell)</t>
@@ -1463,6 +1463,9 @@
     <t xml:space="preserve">prot</t>
   </si>
   <si>
+    <t xml:space="preserve">v4c-bc:0000002, v4c-bc:0000003</t>
+  </si>
+  <si>
     <t xml:space="preserve">0000-0001-2345-999 Created concept</t>
   </si>
   <si>
@@ -1481,12 +1484,12 @@
     <t xml:space="preserve">zyme</t>
   </si>
   <si>
+    <t xml:space="preserve">v4c-bc:0000003</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://wikipedia.org/enzyme</t>
   </si>
   <si>
-    <t xml:space="preserve">v4c-bc:0000003</t>
-  </si>
-  <si>
     <t xml:space="preserve">    Esterase</t>
   </si>
   <si>
@@ -1517,12 +1520,6 @@
     <t xml:space="preserve">Broader Matches</t>
   </si>
   <si>
-    <t xml:space="preserve">ext:0000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ext:0000003</t>
-  </si>
-  <si>
     <t xml:space="preserve">Collections</t>
   </si>
   <si>
@@ -1550,54 +1547,7 @@
     <t xml:space="preserve">Collection of terms related to biocatalysis.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc:0000001, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:0000002, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:0000003</t>
-    </r>
+    <t xml:space="preserve">v4c-bc:0000001, v4c-bc:0000002, v4c-bc:0000003</t>
   </si>
   <si>
     <t xml:space="preserve">https://orcid.org/0000-0001-2345-9999 Created collection</t>
@@ -1619,9 +1569,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4c-bc</t>
   </si>
   <si>
     <t xml:space="preserve">https://example.org/voc4cat_biocatalysis/</t>
@@ -1635,7 +1582,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="21">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1777,8 +1724,15 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1806,12 +1760,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
@@ -1909,7 +1857,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="35">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1986,7 +1934,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1998,15 +1946,23 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="20" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="19" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="3" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="24" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2022,7 +1978,19 @@
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2202,9 +2170,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579960</xdr:colOff>
+      <xdr:colOff>580680</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>133200</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2218,8 +2186,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1375920" y="304920"/>
-          <a:ext cx="5917320" cy="1542240"/>
+          <a:off x="1374480" y="304920"/>
+          <a:ext cx="5911920" cy="1542960"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2295,11 +2263,11 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2478,11 +2446,11 @@
   </sheetPr>
   <dimension ref="A1:J1152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -2608,7 +2576,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="16" t="s">
         <v>25</v>
       </c>
@@ -3005,7 +2973,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="16" t="s">
         <v>26</v>
       </c>
@@ -3459,7 +3427,7 @@
       <c r="J88" s="16"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="16" t="s">
         <v>27</v>
       </c>
@@ -3916,7 +3884,7 @@
       <c r="J131" s="16"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="16" t="s">
         <v>29</v>
       </c>
@@ -4040,7 +4008,7 @@
       <c r="J143" s="16"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="17" t="s">
         <v>30</v>
       </c>
@@ -5197,11 +5165,11 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -5288,7 +5256,7 @@
       <c r="A7" s="18" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="B7" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C7" s="20" t="s">
@@ -5302,7 +5270,7 @@
       <c r="A8" s="18" t="s">
         <v>58</v>
       </c>
-      <c r="B8" s="19" t="s">
+      <c r="B8" s="24" t="s">
         <v>55</v>
       </c>
       <c r="C8" s="20" t="s">
@@ -5316,7 +5284,7 @@
       <c r="A9" s="18" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="B9" s="25" t="s">
         <v>60</v>
       </c>
       <c r="C9" s="20" t="s">
@@ -5344,7 +5312,7 @@
       <c r="A11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="B11" s="24" t="s">
         <v>67</v>
       </c>
       <c r="C11" s="20" t="s">
@@ -5358,7 +5326,7 @@
       <c r="A12" s="18" t="s">
         <v>69</v>
       </c>
-      <c r="B12" s="24"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="20" t="s">
         <v>70</v>
       </c>
@@ -6349,9 +6317,6 @@
     <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999 mark doerr"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6369,11 +6334,11 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G3" activeCellId="0" sqref="G3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6383,7 +6348,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="30"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="27"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="23.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="26.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -6392,279 +6357,283 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="C2" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="D2" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="F2" s="27" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="27" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="25" t="s">
+      <c r="H2" s="27" t="s">
         <v>63</v>
       </c>
-      <c r="I2" s="25" t="s">
+      <c r="I2" s="27" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+    <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="28" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="C3" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="26" t="s">
+      <c r="E3" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="F3" s="29" t="s">
         <v>85</v>
       </c>
-      <c r="G3" s="27"/>
-      <c r="H3" s="27" t="s">
+      <c r="G3" s="30" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="27" t="s">
+      <c r="H3" s="29" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="I3" s="29" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="27" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="28" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="26" t="s">
+      <c r="B4" s="29" t="s">
+        <v>90</v>
+      </c>
+      <c r="C4" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D4" s="27" t="s">
-        <v>90</v>
-      </c>
-      <c r="E4" s="26" t="s">
+      <c r="D4" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="E4" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F4" s="27" t="s">
-        <v>91</v>
-      </c>
-      <c r="G4" s="27"/>
-      <c r="H4" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="I4" s="28" t="s">
+      <c r="F4" s="29" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="5" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="26" t="s">
+      <c r="G4" s="30" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="H4" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I4" s="31" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="26" t="s">
+    </row>
+    <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="28" t="s">
+        <v>93</v>
+      </c>
+      <c r="B5" s="29" t="s">
+        <v>95</v>
+      </c>
+      <c r="C5" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="D5" s="27" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" s="26" t="s">
+      <c r="D5" s="29" t="s">
+        <v>96</v>
+      </c>
+      <c r="E5" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="F5" s="27" t="s">
-        <v>96</v>
-      </c>
-      <c r="G5" s="27"/>
-      <c r="H5" s="27" t="s">
-        <v>86</v>
-      </c>
-      <c r="I5" s="27" t="s">
+      <c r="F5" s="29" t="s">
         <v>97</v>
       </c>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="I5" s="29" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
+      <c r="A6" s="32"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="32"/>
+      <c r="F6" s="33"/>
+      <c r="G6" s="33"/>
+      <c r="H6" s="33"/>
+      <c r="I6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="A7" s="32"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="32"/>
+      <c r="F7" s="33"/>
+      <c r="G7" s="33"/>
+      <c r="H7" s="33"/>
+      <c r="I7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="32"/>
+      <c r="F8" s="33"/>
+      <c r="G8" s="33"/>
+      <c r="H8" s="33"/>
+      <c r="I8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
+      <c r="A9" s="32"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="32"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="33"/>
+      <c r="H9" s="33"/>
+      <c r="I9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
+      <c r="A10" s="32"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="32"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="32"/>
+      <c r="F10" s="33"/>
+      <c r="G10" s="33"/>
+      <c r="H10" s="33"/>
+      <c r="I10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="A11" s="32"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="32"/>
+      <c r="F11" s="33"/>
+      <c r="G11" s="33"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="A12" s="32"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="32"/>
+      <c r="F12" s="33"/>
+      <c r="G12" s="33"/>
+      <c r="H12" s="33"/>
+      <c r="I12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="A13" s="32"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="32"/>
+      <c r="F13" s="33"/>
+      <c r="G13" s="33"/>
+      <c r="H13" s="33"/>
+      <c r="I13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+      <c r="A14" s="32"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="32"/>
+      <c r="F14" s="33"/>
+      <c r="G14" s="33"/>
+      <c r="H14" s="33"/>
+      <c r="I14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+      <c r="A15" s="32"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="32"/>
+      <c r="F15" s="33"/>
+      <c r="G15" s="33"/>
+      <c r="H15" s="33"/>
+      <c r="I15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="A16" s="32"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="32"/>
+      <c r="F16" s="33"/>
+      <c r="G16" s="33"/>
+      <c r="H16" s="33"/>
+      <c r="I16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
+      <c r="A17" s="32"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="32"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="32"/>
+      <c r="F17" s="33"/>
+      <c r="G17" s="33"/>
+      <c r="H17" s="33"/>
+      <c r="I17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="A18" s="32"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="32"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="32"/>
+      <c r="F18" s="33"/>
+      <c r="G18" s="33"/>
+      <c r="H18" s="33"/>
+      <c r="I18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
+      <c r="A19" s="32"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="32"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="33"/>
+      <c r="G19" s="33"/>
+      <c r="H19" s="33"/>
+      <c r="I19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
+      <c r="A20" s="32"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="32"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="32"/>
+      <c r="F20" s="33"/>
+      <c r="G20" s="33"/>
+      <c r="H20" s="33"/>
+      <c r="I20" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6693,11 +6662,11 @@
   </sheetPr>
   <dimension ref="A1:F485"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -6705,36 +6674,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="A2" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="25" t="s">
-        <v>99</v>
-      </c>
-      <c r="C2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="C2" s="27" t="s">
         <v>101</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="D2" s="27" t="s">
         <v>102</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>103</v>
       </c>
+      <c r="F2" s="27" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>105</v>
-      </c>
+      <c r="A3" s="32"/>
+      <c r="B3" s="32"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7239,176 +7204,176 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.29"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="27" t="s">
         <v>106</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="25" t="s">
+      <c r="B2" s="27" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="27" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="27" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="25" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="13.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="29" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="B3" s="29" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="29" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="29" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="33"/>
+      <c r="B4" s="33"/>
+      <c r="C4" s="33"/>
+      <c r="D4" s="33"/>
+      <c r="E4" s="33"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="A5" s="33"/>
+      <c r="B5" s="33"/>
+      <c r="C5" s="33"/>
+      <c r="D5" s="33"/>
+      <c r="E5" s="33"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="A6" s="33"/>
+      <c r="B6" s="33"/>
+      <c r="C6" s="33"/>
+      <c r="D6" s="33"/>
+      <c r="E6" s="33"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="33"/>
+      <c r="B7" s="33"/>
+      <c r="C7" s="33"/>
+      <c r="D7" s="33"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="33"/>
+      <c r="B10" s="33"/>
+      <c r="C10" s="33"/>
+      <c r="D10" s="33"/>
+      <c r="E10" s="33"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="A11" s="33"/>
+      <c r="B11" s="33"/>
+      <c r="C11" s="33"/>
+      <c r="D11" s="33"/>
+      <c r="E11" s="33"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="33"/>
+      <c r="B12" s="33"/>
+      <c r="C12" s="33"/>
+      <c r="D12" s="33"/>
+      <c r="E12" s="33"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="33"/>
+      <c r="B13" s="33"/>
+      <c r="C13" s="33"/>
+      <c r="D13" s="33"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="A14" s="33"/>
+      <c r="B14" s="33"/>
+      <c r="C14" s="33"/>
+      <c r="D14" s="33"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="A15" s="33"/>
+      <c r="B15" s="33"/>
+      <c r="C15" s="33"/>
+      <c r="D15" s="33"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="A16" s="33"/>
+      <c r="B16" s="33"/>
+      <c r="C16" s="33"/>
+      <c r="D16" s="33"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="A17" s="33"/>
+      <c r="B17" s="33"/>
+      <c r="C17" s="33"/>
+      <c r="D17" s="33"/>
+      <c r="E17" s="33"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="A18" s="33"/>
+      <c r="B18" s="33"/>
+      <c r="C18" s="33"/>
+      <c r="D18" s="33"/>
+      <c r="E18" s="33"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="A19" s="33"/>
+      <c r="B19" s="33"/>
+      <c r="C19" s="33"/>
+      <c r="D19" s="33"/>
+      <c r="E19" s="33"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="A20" s="33"/>
+      <c r="B20" s="33"/>
+      <c r="C20" s="33"/>
+      <c r="D20" s="33"/>
+      <c r="E20" s="33"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -7434,95 +7399,99 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.57421875" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="27" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="27" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="25" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="34" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
+      <c r="B2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="34" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="B3" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="34" t="s">
+        <v>37</v>
+      </c>
+      <c r="B4" s="34" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>124</v>
-      </c>
-    </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29"/>
+      <c r="A5" s="34"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
+      <c r="A6" s="34"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29"/>
+      <c r="A7" s="34"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29"/>
+      <c r="A8" s="34"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
+      <c r="A9" s="34"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29"/>
+      <c r="A10" s="34"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
+      <c r="A11" s="34"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29"/>
+      <c r="A12" s="34"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="34"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
+      <c r="A14" s="34"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
+      <c r="A15" s="34"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29"/>
+      <c r="A16" s="34"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29"/>
+      <c r="A17" s="34"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29"/>
+      <c r="A18" s="34"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
+      <c r="A19" s="34"/>
     </row>
   </sheetData>
-  <dataValidations count="1">
-    <dataValidation allowBlank="true" error="A prefix may not end with a colon(:)!" errorStyle="stop" errorTitle="Prefix ends with colon" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A19" type="custom">
+  <dataValidations count="2">
+    <dataValidation allowBlank="true" error="A prefix may not end with a colon(:)!" errorStyle="stop" errorTitle="Prefix ends with colon" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A2:A3 A5:A19" type="custom">
+      <formula1>ISERROR(SEARCH(":",A2))</formula1>
+      <formula2>0</formula2>
+    </dataValidation>
+    <dataValidation allowBlank="true" error="A prefix may not end with a colon(:)!" errorStyle="stop" errorTitle="Prefix ends with colon" operator="between" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="A4" type="custom">
       <formula1>ISERROR(SEARCH(":",A2))</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -7530,7 +7499,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://example.org/test/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://w3id.org/nfdi4cat/voc4cat_"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://example.org/"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://example.org/voc4cat_biocatalysis/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>

</xml_diff>

<commit_message>
fix: re-generated spreadsheet from original template
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="5"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -78,12 +78,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
   <si>
-    <t xml:space="preserve">0.4.4</t>
+    <t xml:space="preserve">0.4.3</t>
   </si>
   <si>
     <t xml:space="preserve">revision</t>
@@ -388,7 +388,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+      <t xml:space="preserve"> = A ROR ID, an ORCID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
 </t>
     </r>
     <r>
@@ -410,7 +410,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organisation, e.g. "NFDI4Cat". 
+      <t xml:space="preserve"> = A ROR ID or a predefined short-ID-string for an organization, e.g. "NFDI4Cat". 
 </t>
     </r>
     <r>
@@ -422,7 +422,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Note: Either the abbreviation for an organisation or its URI can be given. The organisation abbreviation is validated against a predefined list of organisations. If you miss an organisation, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).
+      <t xml:space="preserve">Note: Either the abbreviation for an organization or its URI can be given. The organization abbreviation is validated against a predefined list of organizations. If you miss an organization, create an issue at https://github.com/nfdi4cat/vocexcel/issues and ask for addition (or just use a ROR ID!).
 </t>
     </r>
     <r>
@@ -581,7 +581,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organisation system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
+      <t xml:space="preserve">A concept according to SKOS is a unit of thought, idea, meaning, or category of an object or event which underlies a knowledge organization system. This sheet collects concept descriptions, (optionally) their translations to other languages, simple broader/ narrower relations between the concepts and provenance information.
 </t>
     </r>
     <r>
@@ -1237,7 +1237,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">This sheet is for defining a mapping between short pefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
+      <t xml:space="preserve">This sheet is for defining a mapping between short prefixes and namespaces which are the basis for using "compact URI" also called "CURIE". For more on compact URIs, see https://www.w3.org/TR/2010/NOTE-curie-20101216/
 Example: http://example.org/1, http://example.org/2, http://example.org/3</t>
     </r>
     <r>
@@ -1259,7 +1259,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve"> Instead of manually typing out these examples, you can add in the Prefix Sheet a "ex" as Prefix, and "http://example.org/" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
+      <t xml:space="preserve"> Instead of manually typing out said examples, you can add in the Prefix Sheet a "ex" as Prefix, and "http://example.org/" as the corresponding namespace. Then instead of writing the whole IRI, it is possible to write "ex:1, ex:2, ex:3".
 </t>
     </r>
     <r>
@@ -1271,7 +1271,7 @@
         <family val="2"/>
         <charset val="1"/>
       </rPr>
-      <t xml:space="preserve">Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE, a colon is used to separate the prefix from the suffix-part of the IRI.</t>
+      <t xml:space="preserve">Note: In the Prefix Sheet the Prefix must be entered without a colon at the end. Only when the prefix is used in CURIE a colon is used to separate the prefix from the suffix-part of the IRI.</t>
     </r>
   </si>
   <si>
@@ -1328,7 +1328,7 @@
     <t xml:space="preserve">Title*</t>
   </si>
   <si>
-    <t xml:space="preserve">Voc4Cat-BioCatalysis</t>
+    <t xml:space="preserve">A test vocabulary for the voc4cat biocatalysis</t>
   </si>
   <si>
     <t xml:space="preserve">Title of the vocabulary</t>
@@ -1340,7 +1340,7 @@
     <t xml:space="preserve">Description*</t>
   </si>
   <si>
-    <t xml:space="preserve">A test vocabulary for the voc4cat biocatalysis</t>
+    <t xml:space="preserve">A test vocabulary for the voc4cat biocatalysis </t>
   </si>
   <si>
     <t xml:space="preserve">General description of the vocabulary</t>
@@ -1349,9 +1349,6 @@
     <t xml:space="preserve">Created Date*</t>
   </si>
   <si>
-    <t xml:space="preserve">2023/12/12</t>
-  </si>
-  <si>
     <t xml:space="preserve">Date of creation</t>
   </si>
   <si>
@@ -1385,7 +1382,7 @@
     <t xml:space="preserve">Version</t>
   </si>
   <si>
-    <t xml:space="preserve">V2023-12-12</t>
+    <t xml:space="preserve">V2024-02-21</t>
   </si>
   <si>
     <t xml:space="preserve">Version specifier for the vocabulary (or empty cell)</t>
@@ -1397,7 +1394,7 @@
     <t xml:space="preserve">Provenance*</t>
   </si>
   <si>
-    <t xml:space="preserve">https://orcid.org/0000-0001-2345-9999 mark doerr</t>
+    <t xml:space="preserve">https://orcid.org/0000-0003-3270-6895 Mark Doerr</t>
   </si>
   <si>
     <t xml:space="preserve">A note on the Vocabulary source</t>
@@ -1406,7 +1403,7 @@
     <t xml:space="preserve">Custodian</t>
   </si>
   <si>
-    <t xml:space="preserve">mark doerr (orcid:0000-0001-2345-9999)</t>
+    <t xml:space="preserve">Mark Doerr (orcid:0000-0003-3270-6895)</t>
   </si>
   <si>
     <t xml:space="preserve">Vocabulary Content Manager</t>
@@ -1463,7 +1460,7 @@
     <t xml:space="preserve">prot</t>
   </si>
   <si>
-    <t xml:space="preserve">0000-0001-2345-999 Created concept</t>
+    <t xml:space="preserve">0000-0003-3270-6895 Created concept</t>
   </si>
   <si>
     <t xml:space="preserve">https://wikipedia.org/protein</t>
@@ -1481,6 +1478,9 @@
     <t xml:space="preserve">zyme</t>
   </si>
   <si>
+    <t xml:space="preserve">0001-0003-3270-6895 Created concept</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://wikipedia.org/enzyme</t>
   </si>
   <si>
@@ -1496,6 +1496,9 @@
     <t xml:space="preserve">lipase</t>
   </si>
   <si>
+    <t xml:space="preserve">0002-0003-3270-6895 Created concept</t>
+  </si>
+  <si>
     <t xml:space="preserve">https://wikipedia.org/esterase</t>
   </si>
   <si>
@@ -1517,12 +1520,6 @@
     <t xml:space="preserve">Broader Matches</t>
   </si>
   <si>
-    <t xml:space="preserve">ext:0000001</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ext:0000003</t>
-  </si>
-  <si>
     <t xml:space="preserve">Collections</t>
   </si>
   <si>
@@ -1550,57 +1547,10 @@
     <t xml:space="preserve">Collection of terms related to biocatalysis.</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc:0000001, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:0000002, </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">v4c-bc</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color rgb="FF000000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">:0000003</t>
-    </r>
-  </si>
-  <si>
-    <t xml:space="preserve">https://orcid.org/0000-0001-2345-9999 Created collection</t>
+    <t xml:space="preserve">v4c-bc:0000001, v4c-bc:0000002, v4c-bc:0000003</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://orcid.org/0002-0003-3270-6895 Created collection</t>
   </si>
   <si>
     <t xml:space="preserve">Prefix</t>
@@ -1619,12 +1569,6 @@
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_</t>
-  </si>
-  <si>
-    <t xml:space="preserve">v4c-bc</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://example.org/voc4cat_biocatalysis/</t>
   </si>
 </sst>
 </file>
@@ -1635,7 +1579,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1771,14 +1715,8 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
-  <fills count="7">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1806,12 +1744,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFE699"/>
-        <bgColor rgb="FFFFF2CC"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFFF"/>
         <bgColor rgb="FFFFF2CC"/>
       </patternFill>
     </fill>
@@ -1909,7 +1841,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1986,7 +1918,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="1" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -1998,15 +1930,15 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="6" borderId="3" xfId="22" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="22" applyFont="false" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="6" borderId="3" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="24" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2023,6 +1955,14 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2202,9 +2142,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579960</xdr:colOff>
+      <xdr:colOff>580320</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132840</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2218,8 +2158,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1375920" y="304920"/>
-          <a:ext cx="5917320" cy="1542240"/>
+          <a:off x="1375200" y="304920"/>
+          <a:ext cx="5914440" cy="1542600"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2295,11 +2235,11 @@
   </sheetPr>
   <dimension ref="A11:L31"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B14" activeCellId="0" sqref="B14"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2478,11 +2418,11 @@
   </sheetPr>
   <dimension ref="A1:J1152"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A122" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B12" activeCellId="0" sqref="B12"/>
+    <sheetView showFormulas="false" showGridLines="false" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -2608,7 +2548,7 @@
       <c r="I11" s="13"/>
       <c r="J11" s="13"/>
     </row>
-    <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B12" s="16" t="s">
         <v>25</v>
       </c>
@@ -3005,7 +2945,7 @@
       <c r="I47" s="13"/>
       <c r="J47" s="13"/>
     </row>
-    <row r="48" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B48" s="16" t="s">
         <v>26</v>
       </c>
@@ -3459,7 +3399,7 @@
       <c r="J88" s="16"/>
     </row>
     <row r="89" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="90" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="90" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B90" s="16" t="s">
         <v>27</v>
       </c>
@@ -3916,7 +3856,7 @@
       <c r="J131" s="16"/>
     </row>
     <row r="132" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="133" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="133" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B133" s="16" t="s">
         <v>29</v>
       </c>
@@ -4040,7 +3980,7 @@
       <c r="J143" s="16"/>
     </row>
     <row r="144" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="145" customFormat="false" ht="13.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="145" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B145" s="17" t="s">
         <v>30</v>
       </c>
@@ -5197,11 +5137,11 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -5260,81 +5200,81 @@
       <c r="A5" s="18" t="s">
         <v>47</v>
       </c>
-      <c r="B5" s="23" t="s">
+      <c r="B5" s="23" t="n">
+        <v>45343</v>
+      </c>
+      <c r="C5" s="20" t="s">
         <v>48</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="D5" s="21" t="s">
         <v>49</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
+        <v>50</v>
+      </c>
+      <c r="B6" s="23" t="n">
+        <v>45343</v>
+      </c>
+      <c r="C6" s="20" t="s">
         <v>51</v>
       </c>
-      <c r="B6" s="23" t="s">
-        <v>48</v>
-      </c>
-      <c r="C6" s="20" t="s">
+      <c r="D6" s="21" t="s">
         <v>52</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
+        <v>53</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>54</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>55</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="21" t="s">
         <v>56</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>58</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>59</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="C9" s="20" t="s">
         <v>60</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="21" t="s">
         <v>61</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>63</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="20" t="s">
         <v>64</v>
-      </c>
-      <c r="C10" s="20" t="s">
-        <v>65</v>
       </c>
       <c r="D10" s="21" t="s">
         <v>43</v>
@@ -5342,28 +5282,28 @@
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
+        <v>65</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>66</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>67</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>68</v>
-      </c>
       <c r="D11" s="21" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="20" t="s">
+        <v>69</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>70</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6349,9 +6289,6 @@
     <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999 mark doerr"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6369,11 +6306,11 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I6" activeCellId="0" sqref="I6"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6388,93 +6325,93 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>72</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
+        <v>62</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="H2" s="25" t="s">
-        <v>63</v>
-      </c>
-      <c r="I2" s="25" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="26" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
+      <c r="B3" s="27" t="s">
         <v>81</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>83</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>84</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>85</v>
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>86</v>
       </c>
-      <c r="I3" s="27" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="26" t="s">
         <v>87</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="26" t="s">
+      <c r="B4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>89</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="E4" s="26" t="s">
+        <v>82</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>90</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>83</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>91</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="I4" s="28" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="27.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
         <v>93</v>
       </c>
@@ -6482,189 +6419,189 @@
         <v>94</v>
       </c>
       <c r="C5" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D5" s="27" t="s">
         <v>95</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F5" s="27" t="s">
         <v>96</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27" t="s">
-        <v>86</v>
+        <v>97</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="26"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="26"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="26"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="27"/>
-      <c r="I6" s="27"/>
+      <c r="A6" s="29"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="29"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="29"/>
+      <c r="F6" s="30"/>
+      <c r="G6" s="30"/>
+      <c r="H6" s="30"/>
+      <c r="I6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="26"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="26"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="26"/>
-      <c r="F7" s="27"/>
-      <c r="G7" s="27"/>
-      <c r="H7" s="27"/>
-      <c r="I7" s="27"/>
+      <c r="A7" s="29"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="29"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="29"/>
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="30"/>
+      <c r="I7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="26"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="26"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="27"/>
-      <c r="G8" s="27"/>
-      <c r="H8" s="27"/>
-      <c r="I8" s="27"/>
+      <c r="A8" s="29"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="29"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="29"/>
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="30"/>
+      <c r="I8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="26"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="26"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="27"/>
-      <c r="H9" s="27"/>
-      <c r="I9" s="27"/>
+      <c r="A9" s="29"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="29"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="29"/>
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="30"/>
+      <c r="I9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="26"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="26"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
+      <c r="A10" s="29"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="29"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="29"/>
+      <c r="F10" s="30"/>
+      <c r="G10" s="30"/>
+      <c r="H10" s="30"/>
+      <c r="I10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="26"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="26"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="27"/>
-      <c r="G11" s="27"/>
-      <c r="H11" s="27"/>
-      <c r="I11" s="27"/>
+      <c r="A11" s="29"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="29"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
+      <c r="I11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="26"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="27"/>
-      <c r="G12" s="27"/>
-      <c r="H12" s="27"/>
-      <c r="I12" s="27"/>
+      <c r="A12" s="29"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="29"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="29"/>
+      <c r="F12" s="30"/>
+      <c r="G12" s="30"/>
+      <c r="H12" s="30"/>
+      <c r="I12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="26"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="26"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="26"/>
-      <c r="F13" s="27"/>
-      <c r="G13" s="27"/>
-      <c r="H13" s="27"/>
-      <c r="I13" s="27"/>
+      <c r="A13" s="29"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="29"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="29"/>
+      <c r="F13" s="30"/>
+      <c r="G13" s="30"/>
+      <c r="H13" s="30"/>
+      <c r="I13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="26"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="26"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="26"/>
-      <c r="F14" s="27"/>
-      <c r="G14" s="27"/>
-      <c r="H14" s="27"/>
-      <c r="I14" s="27"/>
+      <c r="A14" s="29"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="29"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="29"/>
+      <c r="F14" s="30"/>
+      <c r="G14" s="30"/>
+      <c r="H14" s="30"/>
+      <c r="I14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="26"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="26"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="27"/>
-      <c r="I15" s="27"/>
+      <c r="A15" s="29"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="29"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="29"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="30"/>
+      <c r="I15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="26"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="26"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="27"/>
-      <c r="G16" s="27"/>
-      <c r="H16" s="27"/>
-      <c r="I16" s="27"/>
+      <c r="A16" s="29"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="29"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="29"/>
+      <c r="F16" s="30"/>
+      <c r="G16" s="30"/>
+      <c r="H16" s="30"/>
+      <c r="I16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="26"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="26"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="27"/>
-      <c r="G17" s="27"/>
-      <c r="H17" s="27"/>
-      <c r="I17" s="27"/>
+      <c r="A17" s="29"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="29"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="29"/>
+      <c r="F17" s="30"/>
+      <c r="G17" s="30"/>
+      <c r="H17" s="30"/>
+      <c r="I17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="26"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="26"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="26"/>
-      <c r="F18" s="27"/>
-      <c r="G18" s="27"/>
-      <c r="H18" s="27"/>
-      <c r="I18" s="27"/>
+      <c r="A18" s="29"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="29"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="29"/>
+      <c r="F18" s="30"/>
+      <c r="G18" s="30"/>
+      <c r="H18" s="30"/>
+      <c r="I18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="26"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="26"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="27"/>
-      <c r="G19" s="27"/>
-      <c r="H19" s="27"/>
-      <c r="I19" s="27"/>
+      <c r="A19" s="29"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="29"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="29"/>
+      <c r="F19" s="30"/>
+      <c r="G19" s="30"/>
+      <c r="H19" s="30"/>
+      <c r="I19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="26"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="26"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="26"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="27"/>
-      <c r="I20" s="27"/>
+      <c r="A20" s="29"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="29"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="29"/>
+      <c r="F20" s="30"/>
+      <c r="G20" s="30"/>
+      <c r="H20" s="30"/>
+      <c r="I20" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
@@ -6693,11 +6630,11 @@
   </sheetPr>
   <dimension ref="A1:F485"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A4" activeCellId="0" sqref="A4"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -6705,36 +6642,32 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B2" s="25" t="s">
-        <v>99</v>
+        <v>100</v>
       </c>
       <c r="C2" s="25" t="s">
-        <v>100</v>
+        <v>101</v>
       </c>
       <c r="D2" s="25" t="s">
-        <v>101</v>
+        <v>102</v>
       </c>
       <c r="E2" s="25" t="s">
-        <v>102</v>
+        <v>103</v>
       </c>
       <c r="F2" s="25" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="26" t="s">
-        <v>104</v>
-      </c>
-      <c r="B3" s="26" t="s">
-        <v>105</v>
-      </c>
+      <c r="A3" s="29"/>
+      <c r="B3" s="29"/>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -7239,11 +7172,11 @@
   </sheetPr>
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -7254,165 +7187,165 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>106</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>109</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>110</v>
       </c>
-      <c r="E2" s="25" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="27" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="14.35" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="27" t="s">
+      <c r="B3" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="27" t="s">
         <v>114</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="E3" s="27" t="s">
-        <v>116</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="27"/>
-      <c r="B4" s="27"/>
-      <c r="C4" s="27"/>
-      <c r="D4" s="27"/>
-      <c r="E4" s="27"/>
+      <c r="A4" s="30"/>
+      <c r="B4" s="30"/>
+      <c r="C4" s="30"/>
+      <c r="D4" s="30"/>
+      <c r="E4" s="30"/>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="27"/>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27"/>
-      <c r="D5" s="27"/>
-      <c r="E5" s="27"/>
+      <c r="A5" s="30"/>
+      <c r="B5" s="30"/>
+      <c r="C5" s="30"/>
+      <c r="D5" s="30"/>
+      <c r="E5" s="30"/>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="27"/>
-      <c r="B6" s="27"/>
-      <c r="C6" s="27"/>
-      <c r="D6" s="27"/>
-      <c r="E6" s="27"/>
+      <c r="A6" s="30"/>
+      <c r="B6" s="30"/>
+      <c r="C6" s="30"/>
+      <c r="D6" s="30"/>
+      <c r="E6" s="30"/>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="27"/>
-      <c r="B7" s="27"/>
-      <c r="C7" s="27"/>
-      <c r="D7" s="27"/>
-      <c r="E7" s="27"/>
+      <c r="A7" s="30"/>
+      <c r="B7" s="30"/>
+      <c r="C7" s="30"/>
+      <c r="D7" s="30"/>
+      <c r="E7" s="30"/>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="27"/>
-      <c r="B8" s="27"/>
-      <c r="C8" s="27"/>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27"/>
+      <c r="A8" s="30"/>
+      <c r="B8" s="30"/>
+      <c r="C8" s="30"/>
+      <c r="D8" s="30"/>
+      <c r="E8" s="30"/>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="27"/>
-      <c r="B9" s="27"/>
-      <c r="C9" s="27"/>
-      <c r="D9" s="27"/>
-      <c r="E9" s="27"/>
+      <c r="A9" s="30"/>
+      <c r="B9" s="30"/>
+      <c r="C9" s="30"/>
+      <c r="D9" s="30"/>
+      <c r="E9" s="30"/>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="27"/>
-      <c r="B10" s="27"/>
-      <c r="C10" s="27"/>
-      <c r="D10" s="27"/>
-      <c r="E10" s="27"/>
+      <c r="A10" s="30"/>
+      <c r="B10" s="30"/>
+      <c r="C10" s="30"/>
+      <c r="D10" s="30"/>
+      <c r="E10" s="30"/>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="27"/>
-      <c r="B11" s="27"/>
-      <c r="C11" s="27"/>
-      <c r="D11" s="27"/>
-      <c r="E11" s="27"/>
+      <c r="A11" s="30"/>
+      <c r="B11" s="30"/>
+      <c r="C11" s="30"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="27"/>
-      <c r="B12" s="27"/>
-      <c r="C12" s="27"/>
-      <c r="D12" s="27"/>
-      <c r="E12" s="27"/>
+      <c r="A12" s="30"/>
+      <c r="B12" s="30"/>
+      <c r="C12" s="30"/>
+      <c r="D12" s="30"/>
+      <c r="E12" s="30"/>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="27"/>
-      <c r="B13" s="27"/>
-      <c r="C13" s="27"/>
-      <c r="D13" s="27"/>
-      <c r="E13" s="27"/>
+      <c r="A13" s="30"/>
+      <c r="B13" s="30"/>
+      <c r="C13" s="30"/>
+      <c r="D13" s="30"/>
+      <c r="E13" s="30"/>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="27"/>
-      <c r="B14" s="27"/>
-      <c r="C14" s="27"/>
-      <c r="D14" s="27"/>
-      <c r="E14" s="27"/>
+      <c r="A14" s="30"/>
+      <c r="B14" s="30"/>
+      <c r="C14" s="30"/>
+      <c r="D14" s="30"/>
+      <c r="E14" s="30"/>
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="27"/>
-      <c r="B15" s="27"/>
-      <c r="C15" s="27"/>
-      <c r="D15" s="27"/>
-      <c r="E15" s="27"/>
+      <c r="A15" s="30"/>
+      <c r="B15" s="30"/>
+      <c r="C15" s="30"/>
+      <c r="D15" s="30"/>
+      <c r="E15" s="30"/>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="27"/>
-      <c r="B16" s="27"/>
-      <c r="C16" s="27"/>
-      <c r="D16" s="27"/>
-      <c r="E16" s="27"/>
+      <c r="A16" s="30"/>
+      <c r="B16" s="30"/>
+      <c r="C16" s="30"/>
+      <c r="D16" s="30"/>
+      <c r="E16" s="30"/>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="27"/>
-      <c r="B17" s="27"/>
-      <c r="C17" s="27"/>
-      <c r="D17" s="27"/>
-      <c r="E17" s="27"/>
+      <c r="A17" s="30"/>
+      <c r="B17" s="30"/>
+      <c r="C17" s="30"/>
+      <c r="D17" s="30"/>
+      <c r="E17" s="30"/>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="27"/>
-      <c r="B18" s="27"/>
-      <c r="C18" s="27"/>
-      <c r="D18" s="27"/>
-      <c r="E18" s="27"/>
+      <c r="A18" s="30"/>
+      <c r="B18" s="30"/>
+      <c r="C18" s="30"/>
+      <c r="D18" s="30"/>
+      <c r="E18" s="30"/>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="27"/>
-      <c r="B19" s="27"/>
-      <c r="C19" s="27"/>
-      <c r="D19" s="27"/>
-      <c r="E19" s="27"/>
+      <c r="A19" s="30"/>
+      <c r="B19" s="30"/>
+      <c r="C19" s="30"/>
+      <c r="D19" s="30"/>
+      <c r="E19" s="30"/>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="27"/>
-      <c r="B20" s="27"/>
-      <c r="C20" s="27"/>
-      <c r="D20" s="27"/>
-      <c r="E20" s="27"/>
+      <c r="A20" s="30"/>
+      <c r="B20" s="30"/>
+      <c r="C20" s="30"/>
+      <c r="D20" s="30"/>
+      <c r="E20" s="30"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0000-0001-2345-9999 Created collection"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0002-0003-3270-6895"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7434,91 +7367,86 @@
   </sheetPr>
   <dimension ref="A1:B19"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="180" zoomScaleNormal="180" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B5" activeCellId="0" sqref="B5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
+        <v>116</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="25" t="s">
+    </row>
+    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A2" s="31" t="s">
         <v>118</v>
       </c>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="29" t="s">
+      <c r="B2" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="B2" s="0" t="s">
+    </row>
+    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="31" t="s">
         <v>120</v>
       </c>
-    </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A3" s="29" t="s">
+      <c r="B3" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B3" s="0" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="29" t="s">
-        <v>123</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>124</v>
-      </c>
+      <c r="A4" s="31"/>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="29"/>
+      <c r="A5" s="31"/>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A6" s="29"/>
+      <c r="A6" s="31"/>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A7" s="29"/>
+      <c r="A7" s="31"/>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A8" s="29"/>
+      <c r="A8" s="31"/>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A9" s="29"/>
+      <c r="A9" s="31"/>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A10" s="29"/>
+      <c r="A10" s="31"/>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A11" s="29"/>
+      <c r="A11" s="31"/>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A12" s="29"/>
+      <c r="A12" s="31"/>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A13" s="29"/>
+      <c r="A13" s="31"/>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A14" s="29"/>
+      <c r="A14" s="31"/>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A15" s="29"/>
+      <c r="A15" s="31"/>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A16" s="29"/>
+      <c r="A16" s="31"/>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A17" s="29"/>
+      <c r="A17" s="31"/>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A18" s="29"/>
+      <c r="A18" s="31"/>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A19" s="29"/>
+      <c r="A19" s="31"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -7530,7 +7458,6 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://example.org/test/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://w3id.org/nfdi4cat/voc4cat_"/>
-    <hyperlink ref="B4" r:id="rId3" display="https://example.org/"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7540,7 +7467,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId4"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: biocat demo spread sheet fixed
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -1316,7 +1316,7 @@
     <t xml:space="preserve">Vocabulary IRI*</t>
   </si>
   <si>
-    <t xml:space="preserve">V4c-bc</t>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_biocat:</t>
   </si>
   <si>
     <t xml:space="preserve">IRI or CURIE for this vocabulary</t>
@@ -1569,6 +1569,12 @@
   </si>
   <si>
     <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_</t>
+  </si>
+  <si>
+    <t xml:space="preserve">v4c-bc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_biocat</t>
   </si>
 </sst>
 </file>
@@ -1579,7 +1585,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="19">
+  <fonts count="20">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1715,6 +1721,12 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1841,7 +1853,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1967,6 +1979,10 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2142,9 +2158,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>580320</xdr:colOff>
+      <xdr:colOff>579960</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132840</xdr:rowOff>
+      <xdr:rowOff>132480</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2158,8 +2174,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1375200" y="304920"/>
-          <a:ext cx="5914440" cy="1542600"/>
+          <a:off x="1375920" y="304920"/>
+          <a:ext cx="5917320" cy="1542240"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2239,7 +2255,7 @@
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2422,7 +2438,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -5138,10 +5154,10 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B11" activeCellId="0" sqref="B11"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -6289,6 +6305,9 @@
     <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" display="https://w3id.org/nfdi4cat/voc4cat_biocat"/>
+  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6307,10 +6326,10 @@
   <dimension ref="A1:I20"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F5" activeCellId="0" sqref="F5"/>
+      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6634,7 +6653,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -7176,13 +7195,13 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="45.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="26.3"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="35.14"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
@@ -7345,7 +7364,7 @@
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0002-0003-3270-6895"/>
+    <hyperlink ref="E3" r:id="rId1" display="https://orcid.org/0002-0003-3270-6895 Created collection"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7368,10 +7387,10 @@
   <dimension ref="A1:B19"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+      <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.58203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
@@ -7401,7 +7420,12 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="31"/>
+      <c r="A4" s="32" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="31"/>
@@ -7458,6 +7482,7 @@
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1" display="https://example.org/test/"/>
     <hyperlink ref="B3" r:id="rId2" display="https://w3id.org/nfdi4cat/voc4cat_"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://w3id.org/nfdi4cat/voc4cat_biocat"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
@@ -7467,7 +7492,7 @@
     <oddFooter/>
   </headerFooter>
   <tableParts>
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
fix: IRI, colon removed
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="137" uniqueCount="124">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -1314,9 +1314,6 @@
   </si>
   <si>
     <t xml:space="preserve">Vocabulary IRI*</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://w3id.org/nfdi4cat/voc4cat_biocat:</t>
   </si>
   <si>
     <t xml:space="preserve">IRI or CURIE for this vocabulary</t>
@@ -1585,7 +1582,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="dd/mm/yyyy"/>
   </numFmts>
-  <fonts count="20">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
@@ -1721,12 +1718,6 @@
       <family val="2"/>
       <charset val="1"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -1853,7 +1844,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="32">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1979,10 +1970,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -2158,9 +2145,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579960</xdr:colOff>
+      <xdr:colOff>579600</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132480</xdr:rowOff>
+      <xdr:rowOff>132120</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2174,8 +2161,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1375920" y="304920"/>
-          <a:ext cx="5917320" cy="1542240"/>
+          <a:off x="1376640" y="304920"/>
+          <a:ext cx="5919840" cy="1541880"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2255,7 +2242,7 @@
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2438,7 +2425,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -5154,10 +5141,10 @@
   <dimension ref="A1:D994"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
+      <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -5174,152 +5161,150 @@
       <c r="A2" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="19"/>
+      <c r="C2" s="20" t="s">
         <v>37</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="D2" s="21" t="s">
         <v>38</v>
-      </c>
-      <c r="D2" s="21" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="39" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="18" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="22" t="s">
+      <c r="C3" s="20" t="s">
         <v>41</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="D3" s="21" t="s">
         <v>42</v>
-      </c>
-      <c r="D3" s="21" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="66.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="19" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="C4" s="20" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="20" t="s">
-        <v>46</v>
-      </c>
       <c r="D4" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="27" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="18" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B5" s="23" t="n">
         <v>45343</v>
       </c>
       <c r="C5" s="20" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="21" t="s">
         <v>48</v>
-      </c>
-      <c r="D5" s="21" t="s">
-        <v>49</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="29.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="18" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B6" s="23" t="n">
         <v>45343</v>
       </c>
       <c r="C6" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="D6" s="21" t="s">
         <v>51</v>
-      </c>
-      <c r="D6" s="21" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="27.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="18" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7" s="19" t="s">
         <v>53</v>
       </c>
-      <c r="B7" s="19" t="s">
+      <c r="C7" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="D7" s="21" t="s">
         <v>55</v>
-      </c>
-      <c r="D7" s="21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="18" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B8" s="19" t="s">
+        <v>53</v>
+      </c>
+      <c r="C8" s="20" t="s">
         <v>54</v>
       </c>
-      <c r="C8" s="20" t="s">
+      <c r="D8" s="21" t="s">
         <v>55</v>
-      </c>
-      <c r="D8" s="21" t="s">
-        <v>56</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B9" s="24" t="s">
         <v>58</v>
       </c>
-      <c r="B9" s="24" t="s">
+      <c r="C9" s="20" t="s">
         <v>59</v>
       </c>
-      <c r="C9" s="20" t="s">
+      <c r="D9" s="21" t="s">
         <v>60</v>
-      </c>
-      <c r="D9" s="21" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="18" t="s">
+        <v>61</v>
+      </c>
+      <c r="B10" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="B10" s="19" t="s">
+      <c r="C10" s="20" t="s">
         <v>63</v>
       </c>
-      <c r="C10" s="20" t="s">
-        <v>64</v>
-      </c>
       <c r="D10" s="21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="21.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="18" t="s">
+        <v>64</v>
+      </c>
+      <c r="B11" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="B11" s="19" t="s">
+      <c r="C11" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C11" s="20" t="s">
-        <v>67</v>
-      </c>
       <c r="D11" s="21" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="31.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="18" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B12" s="24"/>
       <c r="C12" s="20" t="s">
+        <v>68</v>
+      </c>
+      <c r="D12" s="21" t="s">
         <v>69</v>
-      </c>
-      <c r="D12" s="21" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
@@ -6305,9 +6290,6 @@
     <row r="993" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="994" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B2" r:id="rId1" display="https://w3id.org/nfdi4cat/voc4cat_biocat"/>
-  </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
   <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -6329,7 +6311,7 @@
       <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6344,117 +6326,117 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="30" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>71</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="F2" s="25" t="s">
+      <c r="G2" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="H2" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="I2" s="25" t="s">
         <v>78</v>
-      </c>
-      <c r="H2" s="25" t="s">
-        <v>62</v>
-      </c>
-      <c r="I2" s="25" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="26" t="s">
+        <v>79</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>80</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="C3" s="26" t="s">
+      <c r="D3" s="27" t="s">
         <v>82</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="27" t="s">
         <v>83</v>
-      </c>
-      <c r="E3" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F3" s="27" t="s">
-        <v>84</v>
       </c>
       <c r="G3" s="27"/>
       <c r="H3" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I3" s="27" t="s">
         <v>85</v>
-      </c>
-      <c r="I3" s="27" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="26" t="s">
+        <v>86</v>
+      </c>
+      <c r="B4" s="27" t="s">
         <v>87</v>
       </c>
-      <c r="B4" s="27" t="s">
+      <c r="C4" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4" s="27" t="s">
         <v>88</v>
       </c>
-      <c r="C4" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D4" s="27" t="s">
+      <c r="E4" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F4" s="27" t="s">
         <v>89</v>
-      </c>
-      <c r="E4" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F4" s="27" t="s">
-        <v>90</v>
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27" t="s">
+        <v>90</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>91</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>92</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>93</v>
       </c>
-      <c r="B5" s="27" t="s">
+      <c r="C5" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="D5" s="27" t="s">
         <v>94</v>
       </c>
-      <c r="C5" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="D5" s="27" t="s">
+      <c r="E5" s="26" t="s">
+        <v>81</v>
+      </c>
+      <c r="F5" s="27" t="s">
         <v>95</v>
-      </c>
-      <c r="E5" s="26" t="s">
-        <v>82</v>
-      </c>
-      <c r="F5" s="27" t="s">
-        <v>96</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27" t="s">
+        <v>96</v>
+      </c>
+      <c r="I5" s="27" t="s">
         <v>97</v>
-      </c>
-      <c r="I5" s="27" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6653,7 +6635,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -6661,27 +6643,27 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>101</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>102</v>
       </c>
-      <c r="E2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>103</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>104</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7195,7 +7177,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -7206,41 +7188,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>105</v>
+      </c>
+      <c r="B2" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="C2" s="25" t="s">
         <v>107</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>108</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>109</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>110</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="B3" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="C3" s="27" t="s">
         <v>112</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="D3" s="27" t="s">
         <v>113</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>114</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>115</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7390,41 +7372,41 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5859375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
+        <v>115</v>
+      </c>
+      <c r="B1" s="25" t="s">
         <v>116</v>
-      </c>
-      <c r="B1" s="25" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
+        <v>117</v>
+      </c>
+      <c r="B2" s="0" t="s">
         <v>118</v>
-      </c>
-      <c r="B2" s="0" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
+        <v>119</v>
+      </c>
+      <c r="B3" s="0" t="s">
         <v>120</v>
       </c>
-      <c r="B3" s="0" t="s">
+    </row>
+    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="31" t="s">
         <v>121</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A4" s="32" t="s">
+      <c r="B4" s="0" t="s">
         <v>122</v>
-      </c>
-      <c r="B4" s="0" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
fix: Provenance ORCID fixed
</commit_message>
<xml_diff>
--- a/inbox-excel-vocabs/biocatalysis_demo.xlsx
+++ b/inbox-excel-vocabs/biocatalysis_demo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Introduction" sheetId="1" state="visible" r:id="rId2"/>
@@ -78,7 +78,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="121">
   <si>
     <t xml:space="preserve">Template version</t>
   </si>
@@ -1475,9 +1475,6 @@
     <t xml:space="preserve">zyme</t>
   </si>
   <si>
-    <t xml:space="preserve">0001-0003-3270-6895 Created concept</t>
-  </si>
-  <si>
     <t xml:space="preserve">https://wikipedia.org/enzyme</t>
   </si>
   <si>
@@ -1491,9 +1488,6 @@
   </si>
   <si>
     <t xml:space="preserve">lipase</t>
-  </si>
-  <si>
-    <t xml:space="preserve">0002-0003-3270-6895 Created concept</t>
   </si>
   <si>
     <t xml:space="preserve">https://wikipedia.org/esterase</t>
@@ -2145,9 +2139,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>579600</xdr:colOff>
+      <xdr:colOff>579240</xdr:colOff>
       <xdr:row>9</xdr:row>
-      <xdr:rowOff>132120</xdr:rowOff>
+      <xdr:rowOff>131760</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2161,8 +2155,8 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="1376640" y="304920"/>
-          <a:ext cx="5919840" cy="1541880"/>
+          <a:off x="1377360" y="304920"/>
+          <a:ext cx="5922720" cy="1541520"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -2242,7 +2236,7 @@
       <selection pane="topLeft" activeCell="J12" activeCellId="0" sqref="J12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="9.28"/>
   </cols>
@@ -2425,7 +2419,7 @@
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12"/>
@@ -5140,11 +5134,11 @@
   </sheetPr>
   <dimension ref="A1:D994"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="18.43"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="64.14"/>
@@ -6307,11 +6301,11 @@
   </sheetPr>
   <dimension ref="A1:I20"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A5" activeCellId="0" sqref="A5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H10" activeCellId="0" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="20.85"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.85"/>
@@ -6406,37 +6400,37 @@
       </c>
       <c r="G4" s="27"/>
       <c r="H4" s="27" t="s">
+        <v>84</v>
+      </c>
+      <c r="I4" s="28" t="s">
         <v>90</v>
-      </c>
-      <c r="I4" s="28" t="s">
-        <v>91</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="26" t="s">
+        <v>91</v>
+      </c>
+      <c r="B5" s="27" t="s">
         <v>92</v>
-      </c>
-      <c r="B5" s="27" t="s">
-        <v>93</v>
       </c>
       <c r="C5" s="26" t="s">
         <v>81</v>
       </c>
       <c r="D5" s="27" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E5" s="26" t="s">
         <v>81</v>
       </c>
       <c r="F5" s="27" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="G5" s="27"/>
       <c r="H5" s="27" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
       <c r="I5" s="27" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6635,7 +6629,7 @@
       <selection pane="topLeft" activeCell="A3" activeCellId="0" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="50.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="2" style="0" width="25.15"/>
@@ -6643,7 +6637,7 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6651,19 +6645,19 @@
         <v>71</v>
       </c>
       <c r="B2" s="25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C2" s="25" t="s">
+        <v>98</v>
+      </c>
+      <c r="D2" s="25" t="s">
         <v>99</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>100</v>
       </c>
-      <c r="D2" s="25" t="s">
+      <c r="F2" s="25" t="s">
         <v>101</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>102</v>
-      </c>
-      <c r="F2" s="25" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7177,7 +7171,7 @@
       <selection pane="topLeft" activeCell="E3" activeCellId="0" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="23.72"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="16.85"/>
@@ -7188,41 +7182,41 @@
   <sheetData>
     <row r="1" customFormat="false" ht="35.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A1" s="12" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="25" t="s">
+        <v>103</v>
+      </c>
+      <c r="B2" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="C2" s="25" t="s">
         <v>105</v>
       </c>
-      <c r="B2" s="25" t="s">
+      <c r="D2" s="25" t="s">
         <v>106</v>
       </c>
-      <c r="C2" s="25" t="s">
+      <c r="E2" s="25" t="s">
         <v>107</v>
-      </c>
-      <c r="D2" s="25" t="s">
-        <v>108</v>
-      </c>
-      <c r="E2" s="25" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="26.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="27" t="s">
+        <v>108</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>109</v>
+      </c>
+      <c r="C3" s="27" t="s">
         <v>110</v>
       </c>
-      <c r="B3" s="27" t="s">
+      <c r="D3" s="27" t="s">
         <v>111</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>112</v>
-      </c>
-      <c r="D3" s="27" t="s">
-        <v>113</v>
-      </c>
-      <c r="E3" s="27" t="s">
-        <v>114</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7372,41 +7366,41 @@
       <selection pane="topLeft" activeCell="B4" activeCellId="0" sqref="B4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.59375" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6015625" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="43.71"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="25" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B1" s="25" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="31" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="31" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="31" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">

</xml_diff>